<commit_message>
Finished routing except ground plane
</commit_message>
<xml_diff>
--- a/BOM_SPI_Switch_Board.xlsx
+++ b/BOM_SPI_Switch_Board.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="260" windowWidth="21500" windowHeight="21580" tabRatio="500"/>
+    <workbookView xWindow="200" yWindow="260" windowWidth="21500" windowHeight="21580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="90">
   <si>
     <t>2512 (6432 Metric)</t>
   </si>
@@ -95,9 +95,6 @@
     <t>UUR1H221MNL1GS</t>
   </si>
   <si>
-    <t>C3, C5, C6</t>
-  </si>
-  <si>
     <t>10 uF</t>
   </si>
   <si>
@@ -290,6 +287,32 @@
   </si>
   <si>
     <t>2k Ohm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>10uF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ceramic</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1276-1450-1-ND</t>
+  </si>
+  <si>
+    <t>CL05A106MP5NUNC</t>
+  </si>
+  <si>
+    <t>0402 (1005 Metric)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1, C5</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -297,12 +320,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
@@ -723,7 +740,7 @@
   <dimension ref="A1:X100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1"/>
@@ -738,7 +755,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="29" customHeight="1">
       <c r="A1" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="7"/>
@@ -766,7 +783,7 @@
     </row>
     <row r="2" spans="1:24" ht="12">
       <c r="D2" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2">
         <v>49469585</v>
@@ -791,7 +808,7 @@
     </row>
     <row r="3" spans="1:24" ht="12">
       <c r="D3" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3">
         <v>57341</v>
@@ -934,25 +951,25 @@
     </row>
     <row r="8" spans="1:24">
       <c r="A8" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="G8" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -974,22 +991,22 @@
     </row>
     <row r="9" spans="1:24">
       <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="G9" s="4">
         <v>1</v>
@@ -1014,22 +1031,22 @@
     </row>
     <row r="10" spans="1:24">
       <c r="A10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="G10" s="4">
         <v>1</v>
@@ -1054,22 +1071,22 @@
     </row>
     <row r="11" spans="1:24">
       <c r="A11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="D11" s="4">
         <v>705510037</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G11" s="4">
         <v>2</v>
@@ -1094,22 +1111,22 @@
     </row>
     <row r="12" spans="1:24">
       <c r="A12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="F12" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G12" s="4">
         <v>2</v>
@@ -1134,22 +1151,22 @@
     </row>
     <row r="13" spans="1:24">
       <c r="A13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="F13" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G13" s="4">
         <v>1</v>
@@ -1174,22 +1191,22 @@
     </row>
     <row r="14" spans="1:24">
       <c r="A14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="F14" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G14" s="4">
         <v>1</v>
@@ -1214,22 +1231,22 @@
     </row>
     <row r="15" spans="1:24">
       <c r="A15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="F15" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G15" s="4">
         <v>1</v>
@@ -1254,22 +1271,22 @@
     </row>
     <row r="16" spans="1:24" ht="12">
       <c r="A16" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="D16" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" s="4" t="s">
+      <c r="F16" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="G16" s="4">
         <v>4</v>
@@ -1294,22 +1311,22 @@
     </row>
     <row r="17" spans="1:24" ht="12">
       <c r="A17" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="E17" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="G17" s="4">
         <v>6</v>
@@ -1334,22 +1351,22 @@
     </row>
     <row r="18" spans="1:24" ht="12.75" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="E18" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="G18" s="4">
         <v>1</v>
@@ -1374,22 +1391,22 @@
     </row>
     <row r="19" spans="1:24" ht="12">
       <c r="A19" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="E19" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="G19" s="4">
         <v>2</v>
@@ -1414,10 +1431,10 @@
     </row>
     <row r="20" spans="1:24" ht="12">
       <c r="A20" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>1</v>
@@ -1493,13 +1510,27 @@
       <c r="X21" s="1"/>
     </row>
     <row r="22" spans="1:24" ht="12">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="A22" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G22" s="4">
+        <v>2</v>
+      </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -1518,7 +1549,7 @@
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
     </row>
-    <row r="23" spans="1:24">
+    <row r="23" spans="1:24" ht="12">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -3552,7 +3583,6 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Created fabrication outpute, this is the version I sent to Daniel on Dec 3rd
</commit_message>
<xml_diff>
--- a/BOM_SPI_Switch_Board.xlsx
+++ b/BOM_SPI_Switch_Board.xlsx
@@ -74,9 +74,6 @@
     <t>Manufacturer Part Number</t>
   </si>
   <si>
-    <t>Quantity Per Board</t>
-  </si>
-  <si>
     <t>C7</t>
   </si>
   <si>
@@ -313,6 +310,10 @@
   </si>
   <si>
     <t>C1, C5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qty Per Board</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -740,22 +741,23 @@
   <dimension ref="A1:X100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="5" max="5" width="26.5" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" customWidth="1"/>
-    <col min="7" max="7" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="22.83203125" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="29" customHeight="1">
       <c r="A1" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="7"/>
@@ -783,7 +785,7 @@
     </row>
     <row r="2" spans="1:24" ht="12">
       <c r="D2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E2">
         <v>49469585</v>
@@ -808,7 +810,7 @@
     </row>
     <row r="3" spans="1:24" ht="12">
       <c r="D3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E3">
         <v>57341</v>
@@ -869,7 +871,7 @@
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" ht="12">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -889,7 +891,7 @@
         <v>15</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>16</v>
+        <v>89</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -911,22 +913,22 @@
     </row>
     <row r="7" spans="1:24">
       <c r="A7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="G7" s="4">
         <v>1</v>
@@ -951,22 +953,22 @@
     </row>
     <row r="8" spans="1:24">
       <c r="A8" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="G8" s="4">
         <v>1</v>
@@ -991,22 +993,22 @@
     </row>
     <row r="9" spans="1:24">
       <c r="A9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="G9" s="4">
         <v>1</v>
@@ -1031,22 +1033,22 @@
     </row>
     <row r="10" spans="1:24">
       <c r="A10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="G10" s="4">
         <v>1</v>
@@ -1071,22 +1073,22 @@
     </row>
     <row r="11" spans="1:24">
       <c r="A11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="D11" s="4">
         <v>705510037</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G11" s="4">
         <v>2</v>
@@ -1111,22 +1113,22 @@
     </row>
     <row r="12" spans="1:24">
       <c r="A12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="F12" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G12" s="4">
         <v>2</v>
@@ -1151,22 +1153,22 @@
     </row>
     <row r="13" spans="1:24">
       <c r="A13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="F13" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G13" s="4">
         <v>1</v>
@@ -1191,22 +1193,22 @@
     </row>
     <row r="14" spans="1:24">
       <c r="A14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="F14" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G14" s="4">
         <v>1</v>
@@ -1231,22 +1233,22 @@
     </row>
     <row r="15" spans="1:24">
       <c r="A15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="F15" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G15" s="4">
         <v>1</v>
@@ -1271,22 +1273,22 @@
     </row>
     <row r="16" spans="1:24" ht="12">
       <c r="A16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="D16" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E16" s="4" t="s">
+      <c r="F16" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="G16" s="4">
         <v>4</v>
@@ -1309,24 +1311,24 @@
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
     </row>
-    <row r="17" spans="1:24" ht="12">
+    <row r="17" spans="1:24" ht="36">
       <c r="A17" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="E17" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>76</v>
       </c>
       <c r="G17" s="4">
         <v>6</v>
@@ -1351,22 +1353,22 @@
     </row>
     <row r="18" spans="1:24" ht="12.75" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="E18" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="G18" s="4">
         <v>1</v>
@@ -1391,22 +1393,22 @@
     </row>
     <row r="19" spans="1:24" ht="12">
       <c r="A19" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="E19" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="G19" s="4">
         <v>2</v>
@@ -1429,12 +1431,12 @@
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
     </row>
-    <row r="20" spans="1:24" ht="12">
+    <row r="20" spans="1:24" ht="36">
       <c r="A20" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>82</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>1</v>
@@ -1511,22 +1513,22 @@
     </row>
     <row r="22" spans="1:24" ht="12">
       <c r="A22" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="D22" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E22" s="4" t="s">
+      <c r="F22" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="G22" s="4">
         <v>2</v>
@@ -3578,11 +3580,13 @@
       <c r="X100" s="1"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Replaced decoupling caps for line driver with a larger package. Added smaller resistors for LEDs. Must ensure we never pull over 20mA with this resistor package.
</commit_message>
<xml_diff>
--- a/BOM_SPI_Switch_Board.xlsx
+++ b/BOM_SPI_Switch_Board.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="260" windowWidth="21500" windowHeight="21580" tabRatio="500"/>
+    <workbookView xWindow="160" yWindow="260" windowWidth="24420" windowHeight="22800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,19 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="90">
-  <si>
-    <t>2512 (6432 Metric)</t>
-  </si>
-  <si>
-    <t>1W Resistor</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PT2.0KXCT-ND</t>
-  </si>
-  <si>
-    <t>ERJ-1TYJ202U</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="84">
+  <si>
+    <t>RNCP1206FTD1K50CT-ND</t>
+  </si>
+  <si>
+    <t>RNCP1206FTD1K50</t>
   </si>
   <si>
     <t>RHM1215CT-ND</t>
@@ -283,37 +276,23 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>2k Ohm</t>
+    <t>Qty Per Board</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>C3</t>
+    <t>C1, C3, C5</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>10uF</t>
+    <t>1.5k Ohm</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Ceramic</t>
+    <t>0.5W Resistor</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>1276-1450-1-ND</t>
-  </si>
-  <si>
-    <t>CL05A106MP5NUNC</t>
-  </si>
-  <si>
-    <t>0402 (1005 Metric)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>C1, C5</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qty Per Board</t>
+    <t>1206 (3216 Metric)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -738,18 +717,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:X100"/>
+  <dimension ref="A1:X99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="12.83203125" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
     <col min="6" max="6" width="22.83203125" customWidth="1"/>
     <col min="7" max="7" width="13.83203125" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" customWidth="1"/>
@@ -757,7 +737,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="29" customHeight="1">
       <c r="A1" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="7"/>
@@ -785,7 +765,7 @@
     </row>
     <row r="2" spans="1:24" ht="12">
       <c r="D2" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E2">
         <v>49469585</v>
@@ -810,7 +790,7 @@
     </row>
     <row r="3" spans="1:24" ht="12">
       <c r="D3" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E3">
         <v>57341</v>
@@ -873,25 +853,25 @@
     </row>
     <row r="6" spans="1:24" ht="12">
       <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="G6" s="3" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -913,22 +893,22 @@
     </row>
     <row r="7" spans="1:24">
       <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="G7" s="4">
         <v>1</v>
@@ -953,22 +933,22 @@
     </row>
     <row r="8" spans="1:24">
       <c r="A8" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="G8" s="4">
         <v>1</v>
@@ -993,22 +973,22 @@
     </row>
     <row r="9" spans="1:24">
       <c r="A9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="G9" s="4">
         <v>1</v>
@@ -1033,22 +1013,22 @@
     </row>
     <row r="10" spans="1:24">
       <c r="A10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="D10" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="G10" s="4">
         <v>1</v>
@@ -1073,22 +1053,22 @@
     </row>
     <row r="11" spans="1:24">
       <c r="A11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="D11" s="4">
         <v>705510037</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G11" s="4">
         <v>2</v>
@@ -1113,22 +1093,22 @@
     </row>
     <row r="12" spans="1:24">
       <c r="A12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="F12" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G12" s="4">
         <v>2</v>
@@ -1153,22 +1133,22 @@
     </row>
     <row r="13" spans="1:24">
       <c r="A13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="F13" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G13" s="4">
         <v>1</v>
@@ -1193,22 +1173,22 @@
     </row>
     <row r="14" spans="1:24">
       <c r="A14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="F14" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G14" s="4">
         <v>1</v>
@@ -1231,24 +1211,24 @@
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" ht="12">
       <c r="A15" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="F15" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G15" s="4">
         <v>1</v>
@@ -1273,22 +1253,22 @@
     </row>
     <row r="16" spans="1:24" ht="12">
       <c r="A16" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="D16" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="F16" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="G16" s="4">
         <v>4</v>
@@ -1313,22 +1293,22 @@
     </row>
     <row r="17" spans="1:24" ht="36">
       <c r="A17" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="G17" s="4">
         <v>6</v>
@@ -1353,22 +1333,22 @@
     </row>
     <row r="18" spans="1:24" ht="12.75" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D18" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="F18" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G18" s="4">
         <v>1</v>
@@ -1393,22 +1373,22 @@
     </row>
     <row r="19" spans="1:24" ht="12">
       <c r="A19" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="C19" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G19" s="4">
         <v>2</v>
@@ -1433,22 +1413,22 @@
     </row>
     <row r="20" spans="1:24" ht="36">
       <c r="A20" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>81</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>1</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>3</v>
       </c>
       <c r="G20" s="4">
         <v>9</v>
@@ -1473,22 +1453,22 @@
     </row>
     <row r="21" spans="1:24" ht="12">
       <c r="A21" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G21" s="4">
         <v>1</v>
@@ -1512,27 +1492,13 @@
       <c r="X21" s="1"/>
     </row>
     <row r="22" spans="1:24" ht="12">
-      <c r="A22" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G22" s="4">
-        <v>2</v>
-      </c>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -1551,7 +1517,7 @@
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
     </row>
-    <row r="23" spans="1:24" ht="12">
+    <row r="23" spans="1:24">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -3553,40 +3519,12 @@
       <c r="W99" s="1"/>
       <c r="X99" s="1"/>
     </row>
-    <row r="100" spans="1:24">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
-      <c r="D100" s="1"/>
-      <c r="E100" s="1"/>
-      <c r="F100" s="1"/>
-      <c r="G100" s="1"/>
-      <c r="H100" s="1"/>
-      <c r="I100" s="1"/>
-      <c r="J100" s="1"/>
-      <c r="K100" s="1"/>
-      <c r="L100" s="1"/>
-      <c r="M100" s="1"/>
-      <c r="N100" s="1"/>
-      <c r="O100" s="1"/>
-      <c r="P100" s="1"/>
-      <c r="Q100" s="1"/>
-      <c r="R100" s="1"/>
-      <c r="S100" s="1"/>
-      <c r="T100" s="1"/>
-      <c r="U100" s="1"/>
-      <c r="V100" s="1"/>
-      <c r="W100" s="1"/>
-      <c r="X100" s="1"/>
-    </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
finished the second go at rev1
</commit_message>
<xml_diff>
--- a/BOM_SPI_Switch_Board.xlsx
+++ b/BOM_SPI_Switch_Board.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="260" windowWidth="24420" windowHeight="22800" tabRatio="500"/>
+    <workbookView xWindow="180" yWindow="260" windowWidth="24420" windowHeight="22800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -300,6 +300,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
@@ -720,7 +726,7 @@
   <dimension ref="A1:X99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1"/>
@@ -3525,6 +3531,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>